<commit_message>
Update job postings for 2024-11-29
</commit_message>
<xml_diff>
--- a/yc-daily-post/11-29-2024_post.xlsx
+++ b/yc-daily-post/11-29-2024_post.xlsx
@@ -124,6 +124,24 @@
     <x:t>https://www.ycombinator.com/companies/kapa-ai/jobs/hrFWJfn-research-engineer-applied-ai</x:t>
   </x:si>
   <x:si>
+    <x:t>MixRank (S11)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/98189b51f5b6f25d164e611f2ea6a3c5f972de3f.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data products for sales, marketing, finance, recruiting, and more.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Junior Software Engineer - Remote</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeBR / Remote (BR)Full stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/mixrank/jobs/cFFeoR1-junior-software-engineer-remote</x:t>
+  </x:si>
+  <x:si>
     <x:t>Tivara (S24)</x:t>
   </x:si>
   <x:si>
@@ -142,210 +160,195 @@
     <x:t>https://www.ycombinator.com/companies/tivara/jobs/6Hhb9Oo-founding-product-engineer</x:t>
   </x:si>
   <x:si>
-    <x:t>MixRank (S11)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/98189b51f5b6f25d164e611f2ea6a3c5f972de3f.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Data products for sales, marketing, finance, recruiting, and more.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Junior Software Engineer - Remote</x:t>
+    <x:t>Pump.co (S22)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/7bd441b185f1d0725ac8c35281774ba67b3fdc86.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Costco for cloud is here </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Founding Designer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeSan Francisco, CA, USFrontend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/pump-co/jobs/jyVciZl-founding-designer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Clarion (W24)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/d42943b90f437bd5f4540ef5967011e4865a3427.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Elevate patient communications with conversational AI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Founding Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeNew York, NY, US / Remote (New York, NY, US; San Francisco, CA, US; Austin, TX, US)Full stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/clarion/jobs/oZugxyj-founding-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Attain (W22)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/49382467e2a565f576c3b472c767c5c5095a0c0b.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>One-Stop Shop for Convenience Store Inventory</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeSan Francisco, CA, US / Remote (US)Full stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/attain/jobs/338TqFo-founding-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Juicebox (S22)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/2a2858087cb4a0409dfdf9550fd470d4f1798ec6.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AI-powered talent sourcing for recruiters</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Founding Engineer (2 Openings)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeSan Francisco, CA, USFull stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/juicebox/jobs/zq1mYU4-founding-engineer-2-openings</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rutter (S19)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/58546f561c6a3cd285083ee0d5e1c3c9c285fcb2.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Universal API for commerce and accounting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Software Engineer (Backend)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeNew York, NY, USBackend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/rutter/jobs/IEalyfm-senior-software-engineer-backend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Agave (W22)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/e9bc3a224a6ab03aa39009f5213c25815ae6a7d5.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>API &amp; Data Infrastructure for Construction</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeSan Francisco, CABackend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/agave/jobs/jryB4nr-software-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fieldguide (S20)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/44c799568df44fb4f129df3ebec9417b8d588116.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vertical AI for Audit &amp; Advisory Firms</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Software Engineer, AI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeUS / Remote (US)Full stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/fieldguide/jobs/XqDhcVp-senior-software-engineer-ai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Forage (S21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/23991b3eac1d06368b01c2f9ce5b893ba315f039.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Payments infrastructure for government benefits</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Security Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeRemote - North America / Remote (US; CA; MX)Backend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/forage-2/jobs/fCJyY8D-security-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Luminai (S20)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/5cf2a6787e214eab9a646841d7032f5365ef6f8e.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Luminai helps automate repetitive manual work away from your mission…</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeSan Mateo / San Mateo, CA, US / RemoteFull stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/luminai/jobs/DyTfa8z-software-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Topline Pro (W21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/c43a0f3a8285bc157c443799365f68e59cff1e3c.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Generative AI powered Shopify for home service professionals</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Frontend Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeBoston, MAFrontend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/topline-pro/jobs/BgVeqA9-senior-frontend-software-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FlutterFlow (W21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/3df7b6e09c2fda2538b0426203b84e4e92ca7471.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Application Development Platform (Native Mobile + Web Apps)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Software Engineer - Flutter (United States)</x:t>
   </x:si>
   <x:si>
     <x:t>Full-timeRemoteFull stack</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ycombinator.com/companies/mixrank/jobs/cFFeoR1-junior-software-engineer-remote</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pump.co (S22)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/7bd441b185f1d0725ac8c35281774ba67b3fdc86.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Costco for cloud is here </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Founding Designer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeSan Francisco, CA, USFrontend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/pump-co/jobs/jyVciZl-founding-designer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Clarion (W24)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/d42943b90f437bd5f4540ef5967011e4865a3427.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Elevate patient communications with conversational AI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Founding Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeNew York, NY, US / Remote (New York, NY, US; San Francisco, CA, US; Austin, TX, US)Full stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/clarion/jobs/oZugxyj-founding-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Attain (W22)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/49382467e2a565f576c3b472c767c5c5095a0c0b.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>One-Stop Shop for Convenience Store Inventory</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeSan Francisco, CA, US / Remote (US)Full stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/attain/jobs/338TqFo-founding-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Juicebox (S22)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/2a2858087cb4a0409dfdf9550fd470d4f1798ec6.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AI-powered talent sourcing for recruiters</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Founding Engineer (2 Openings)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeSan Francisco, CA, USFull stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/juicebox/jobs/zq1mYU4-founding-engineer-2-openings</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rutter (S19)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/58546f561c6a3cd285083ee0d5e1c3c9c285fcb2.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Universal API for commerce and accounting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Software Engineer (Backend)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeNew York, NY, USBackend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/rutter/jobs/IEalyfm-senior-software-engineer-backend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Agave (W22)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/e9bc3a224a6ab03aa39009f5213c25815ae6a7d5.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>API &amp; Data Infrastructure for Construction</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeSan Francisco, CABackend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/agave/jobs/jryB4nr-software-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fieldguide (S20)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/44c799568df44fb4f129df3ebec9417b8d588116.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vertical AI for Audit &amp; Advisory Firms</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Software Engineer, AI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeUS / Remote (US)Full stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/fieldguide/jobs/XqDhcVp-senior-software-engineer-ai</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Forage (S21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/23991b3eac1d06368b01c2f9ce5b893ba315f039.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Payments infrastructure for government benefits</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Security Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeRemote - North America / Remote (US; CA; MX)Backend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/forage-2/jobs/fCJyY8D-security-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Luminai (S20)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/5cf2a6787e214eab9a646841d7032f5365ef6f8e.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Luminai helps automate repetitive manual work away from your mission…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeSan Mateo / San Mateo, CA, US / RemoteFull stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/luminai/jobs/DyTfa8z-software-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Topline Pro (W21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/c43a0f3a8285bc157c443799365f68e59cff1e3c.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Generative AI powered Shopify for home service professionals</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Frontend Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeBoston, MAFrontend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/topline-pro/jobs/BgVeqA9-senior-frontend-software-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FlutterFlow (W21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/3df7b6e09c2fda2538b0426203b84e4e92ca7471.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Application Development Platform (Native Mobile + Web Apps)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Software Engineer - Flutter (United States)</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://www.ycombinator.com/companies/flutterflow/jobs/qxAuDS1-software-engineer-flutter-united-states</x:t>
   </x:si>
   <x:si>
@@ -424,13 +427,13 @@
     <x:t>Google-level engineering productivity suite</x:t>
   </x:si>
   <x:si>
-    <x:t>Software engineer, Fullstack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timePalo Alto, CA, USBackend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/aviator/jobs/2fmcI6d-software-engineer-fullstack</x:t>
+    <x:t>Software engineer, Recent grad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timePalo Alto, CA, USFrontend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/aviator/jobs/acPE4OP-software-engineer-recent-grad</x:t>
   </x:si>
   <x:si>
     <x:t>Converge (S23)</x:t>
@@ -457,13 +460,10 @@
     <x:t>The first public safety operating system that eliminates crime.</x:t>
   </x:si>
   <x:si>
-    <x:t>Android Framework Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeAtlanta, GA, US / Remote (Atlanta, GA, US)Embedded systems</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/flock-safety/jobs/3TX1s8L-android-framework-engineer</x:t>
+    <x:t>Fullstack Software Engineer III, Map</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/flock-safety/jobs/MSsjvnJ-fullstack-software-engineer-iii-map</x:t>
   </x:si>
   <x:si>
     <x:t>Prelim (S17)</x:t>
@@ -481,6 +481,24 @@
     <x:t>https://www.ycombinator.com/companies/prelim/jobs/8rmQ2bD-software-engineer-in-test</x:t>
   </x:si>
   <x:si>
+    <x:t>Coulomb AI (S21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/0d176e9e252d68df98f28ada02fca2e0e1f38e49.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Battery Observability Platform for Electric Vehicles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Frontend Developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeBangaloreFrontend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/coulomb-ai/jobs/exGBsfr-senior-frontend-developer</x:t>
+  </x:si>
+  <x:si>
     <x:t>Reworkd (S23)</x:t>
   </x:si>
   <x:si>
@@ -496,24 +514,6 @@
     <x:t>https://www.ycombinator.com/companies/reworkd/jobs/kqP7tsy-senior-backend-software-engineer</x:t>
   </x:si>
   <x:si>
-    <x:t>Coulomb AI (S21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/0d176e9e252d68df98f28ada02fca2e0e1f38e49.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Battery Observability Platform for Electric Vehicles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Frontend Developer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeBangaloreFrontend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/coulomb-ai/jobs/exGBsfr-senior-frontend-developer</x:t>
-  </x:si>
-  <x:si>
     <x:t>SafeBase (S20)</x:t>
   </x:si>
   <x:si>
@@ -523,13 +523,13 @@
     <x:t>Trust Center platform that scales customer security reviews</x:t>
   </x:si>
   <x:si>
-    <x:t>Senior Software Engineer - Full Stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeUS / CA / Remote (US; CA)Full stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/safebase/jobs/fE3Fdca-senior-software-engineer-full-stack</x:t>
+    <x:t>AI Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeUS / CA / Remote (US; CA)Machine learning</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/safebase/jobs/6mZT895-ai-engineer</x:t>
   </x:si>
   <x:si>
     <x:t>Skio (S20)</x:t>
@@ -568,6 +568,24 @@
     <x:t>https://www.ycombinator.com/companies/rinsed/jobs/QRXTiwt-data-analytics-engineer</x:t>
   </x:si>
   <x:si>
+    <x:t>BusinessOnBot (W21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/03c75b785d321bb19fc8ab6c4a6b736e7b35df44.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Automated user acquisition &amp; selling on WhatsApp for businesses</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lead Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeBangalore, IndiaBackend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/businessonbot/jobs/ZEJQDyH-lead-software-engineer</x:t>
+  </x:si>
+  <x:si>
     <x:t>Two Dots (S22)</x:t>
   </x:si>
   <x:si>
@@ -613,13 +631,13 @@
     <x:t>The first prediction market for sports</x:t>
   </x:si>
   <x:si>
-    <x:t>Senior Backend Engineer / Backend Engineer</x:t>
+    <x:t>Frontend Mobile Engineer</x:t>
   </x:si>
   <x:si>
     <x:t>Full-timeNew York, NYFull stack</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ycombinator.com/companies/novig/jobs/yjMXjnW-senior-backend-engineer-backend-engineer</x:t>
+    <x:t>https://www.ycombinator.com/companies/novig/jobs/ibLgITR-frontend-mobile-engineer</x:t>
   </x:si>
   <x:si>
     <x:t>Truss (S21)</x:t>
@@ -673,22 +691,55 @@
     <x:t>https://www.ycombinator.com/companies/blissway/jobs/cep8MsY-electrical-engineer</x:t>
   </x:si>
   <x:si>
-    <x:t>BusinessOnBot (W21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/03c75b785d321bb19fc8ab6c4a6b736e7b35df44.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Automated user acquisition &amp; selling on WhatsApp for businesses</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lead Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeBangalore, IndiaBackend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/businessonbot/jobs/ZEJQDyH-lead-software-engineer</x:t>
+    <x:t>Spellbrush (W18)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/fb441dcc9519c0cc22e2464b6b1c3b1ca462403b.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Making Anime Real</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anime Games - Unity Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeSan Francisco, CA / Tokyo, JP / RemoteFull stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/spellbrush/jobs/SmU4cmU-anime-games-unity-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Axle Health (W21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/48b548fd88ed1c898f2a5e58f8a6edb67f37bd16.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Scheduling and workforce management SaaS for home healthcare providers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Software Engineer I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeLos Angeles, CA, USFull stack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/axle-health/jobs/jcgpaS1-software-engineer-i</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coast (S21)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/65cb3b99fd44f8b43727970a9cb034fbeee5d0df.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sales Demos for API-First Companies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Software Engineer (Product, Design)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/coast/jobs/ms86GPV-software-engineer-product-design</x:t>
   </x:si>
   <x:si>
     <x:t>Helicone (W23)</x:t>
@@ -703,57 +754,6 @@
     <x:t>https://www.ycombinator.com/companies/helicone/jobs/1Ksy3Cv-founding-engineer</x:t>
   </x:si>
   <x:si>
-    <x:t>Spellbrush (W18)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/fb441dcc9519c0cc22e2464b6b1c3b1ca462403b.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Making Anime Real</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Anime Games - Unity Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeSan Francisco, CA / Tokyo, JP / RemoteFull stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/spellbrush/jobs/SmU4cmU-anime-games-unity-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Axle Health (W21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/48b548fd88ed1c898f2a5e58f8a6edb67f37bd16.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Scheduling and workforce management SaaS for home healthcare providers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Software Engineer I</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeLos Angeles, CA, USFull stack</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/axle-health/jobs/jcgpaS1-software-engineer-i</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Coast (S21)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/65cb3b99fd44f8b43727970a9cb034fbeee5d0df.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sales Demos for API-First Companies</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Software Engineer (Product, Design)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/coast/jobs/ms86GPV-software-engineer-product-design</x:t>
-  </x:si>
-  <x:si>
     <x:t>PlayHT (W23)</x:t>
   </x:si>
   <x:si>
@@ -787,6 +787,39 @@
     <x:t>https://www.ycombinator.com/companies/silurian/jobs/vwXNzXx-founding-research-engineer</x:t>
   </x:si>
   <x:si>
+    <x:t>Tamarind Bio (W24)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/9f825e68bedd9d6fae6a9628ae002227d27ab4d2.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Easy to use computational biology tools for drug discovery</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Founding Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/tamarind-bio/jobs/OEkMxsJ-founding-software-engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Seal (S20)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/c7c574f267298b266e49f83004d0138436eb334f.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>All-in-one workspace for companies making regulated products</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Product Engineer (Full-time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-timeEngland, GBBackend</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ycombinator.com/companies/seal-2/jobs/n4byaPm-product-engineer-full-time</x:t>
+  </x:si>
+  <x:si>
     <x:t>Numeral (W23)</x:t>
   </x:si>
   <x:si>
@@ -802,39 +835,6 @@
     <x:t>https://www.ycombinator.com/companies/numeral/jobs/HLVIyAP-software-engineer-product</x:t>
   </x:si>
   <x:si>
-    <x:t>Tamarind Bio (W24)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/9f825e68bedd9d6fae6a9628ae002227d27ab4d2.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Easy to use computational biology tools for drug discovery</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Founding Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/tamarind-bio/jobs/OEkMxsJ-founding-software-engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Seal (S20)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://bookface-images.s3.amazonaws.com/small_logos/c7c574f267298b266e49f83004d0138436eb334f.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>All-in-one workspace for companies making regulated products</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product Engineer (Full-time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full-timeEngland, GBBackend</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ycombinator.com/companies/seal-2/jobs/n4byaPm-product-engineer-full-time</x:t>
-  </x:si>
-  <x:si>
     <x:t>Meticulate (W24)</x:t>
   </x:si>
   <x:si>
@@ -859,7 +859,7 @@
     <x:t>Software Engineer - Fintech</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ycombinator.com/companies/dripos/jobs/bo9NZrL-software-engineer-fintech</x:t>
+    <x:t>https://www.ycombinator.com/companies/dripos/jobs/mxkpl2M-software-engineer-fintech</x:t>
   </x:si>
   <x:si>
     <x:t>Corgi (S24)</x:t>
@@ -1608,147 +1608,147 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="A20" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>80</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="A21" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="A22" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:6">
       <x:c r="A23" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
       <x:c r="A24" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:6">
       <x:c r="A25" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="A26" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
         <x:v>149</x:v>
@@ -1788,27 +1788,27 @@
         <x:v>158</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="A29" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
         <x:v>165</x:v>
@@ -1965,27 +1965,27 @@
         <x:v>210</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="E37" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:6">
       <x:c r="A38" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="E38" s="0" t="s">
         <x:v>217</x:v>
@@ -2025,70 +2025,70 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="E40" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>230</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:6">
       <x:c r="A41" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="D41" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="E41" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F41" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:6">
       <x:c r="A42" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="E42" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F42" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:6">
       <x:c r="A43" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>242</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E43" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
         <x:v>245</x:v>
@@ -2168,27 +2168,27 @@
         <x:v>265</x:v>
       </x:c>
       <x:c r="E47" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:6">
       <x:c r="A48" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="D48" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E48" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F48" s="0" t="s">
         <x:v>272</x:v>
@@ -2228,7 +2228,7 @@
         <x:v>280</x:v>
       </x:c>
       <x:c r="E50" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F50" s="0" t="s">
         <x:v>281</x:v>

</xml_diff>